<commit_message>
add PST and edit analysis
</commit_message>
<xml_diff>
--- a/Analysis/Questionnaire/questionnaire_analysis_results.xlsx
+++ b/Analysis/Questionnaire/questionnaire_analysis_results.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,14 +478,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>R_42Ga7yjlA5oLJCd</t>
+          <t>R_4EEZWAH8SF10F8e</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.8</v>
       </c>
       <c r="D2" t="n">
         <v>15</v>
@@ -505,14 +505,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>R_9j8Niq4DZA1y7Op</t>
+          <t>R_4AKE20ENCrCGxUl</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>0.06666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="D3" t="n">
         <v>15</v>
@@ -532,14 +532,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>R_92Xn58Elv9fCbLJ</t>
+          <t>R_9aZFWvCRMGokDwl</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D4" t="n">
         <v>15</v>
@@ -559,14 +559,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>R_4pWgwYKsPFaTWcp</t>
+          <t>R_4eV7QBpawwD6eOr</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="D5" t="n">
         <v>15</v>
@@ -586,14 +586,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>R_4ELN7Q0714WIXDZ</t>
+          <t>R_91jRA37lX3YUEbP</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="D6" t="n">
         <v>15</v>
@@ -613,14 +613,14 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>R_9fPoQx2VAiJtvot</t>
+          <t>R_4PvVrWZ4ldg9ZuE</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="D7" t="n">
         <v>15</v>
@@ -640,14 +640,14 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>R_4EEZWAH8SF10F8e</t>
+          <t>R_9Y3cXt4ARx4xD6T</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="D8" t="n">
         <v>15</v>
@@ -667,14 +667,14 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>R_4AKE20ENCrCGxUl</t>
+          <t>R_9N32winq5vbF1El</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="D9" t="n">
         <v>15</v>
@@ -694,14 +694,14 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>R_9aZFWvCRMGokDwl</t>
+          <t>R_9uYGNjx9yWaODxD</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="D10" t="n">
         <v>15</v>
@@ -721,14 +721,14 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>R_4eV7QBpawwD6eOr</t>
+          <t>R_9OPvlHXlbPmz754</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="D11" t="n">
         <v>15</v>
@@ -748,14 +748,14 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>R_91jRA37lX3YUEbP</t>
+          <t>R_9x36NNwdNT2QnEB</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="D12" t="n">
         <v>15</v>
@@ -775,14 +775,14 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>R_4PvVrWZ4ldg9ZuE</t>
+          <t>R_4DfI1n39Bzpi2xH</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>1.666666666666667</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="D13" t="n">
         <v>15</v>
@@ -802,14 +802,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>R_9Y3cXt4ARx4xD6T</t>
+          <t>R_9emki3uWpm88jEt</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8666666666666667</v>
+        <v>1.6</v>
       </c>
       <c r="D14" t="n">
         <v>15</v>
@@ -829,14 +829,14 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>R_9N32winq5vbF1El</t>
+          <t>R_91tsT1u49aBUhks</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>1.333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D15" t="n">
         <v>15</v>
@@ -856,14 +856,14 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>R_9uYGNjx9yWaODxD</t>
+          <t>R_9LAP8tEg6HUmoat</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C16" t="n">
-        <v>1.333333333333333</v>
+        <v>1.6</v>
       </c>
       <c r="D16" t="n">
         <v>15</v>
@@ -883,14 +883,14 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>R_9OPvlHXlbPmz754</t>
+          <t>R_4GCVAoEofofJmxX</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C17" t="n">
-        <v>0.06666666666666667</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="D17" t="n">
         <v>15</v>
@@ -910,14 +910,14 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>R_4rHDTNQ0TLPg3iz</t>
+          <t>R_4dtvPF6tKUsY2Dr</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="D18" t="n">
         <v>15</v>
@@ -937,14 +937,14 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>R_9x36NNwdNT2QnEB</t>
+          <t>R_9bTZgIxUTHOBB65</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="D19" t="n">
         <v>15</v>
@@ -964,14 +964,14 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>R_4DfI1n39Bzpi2xH</t>
+          <t>R_4E1hPlVcrRYDEgI</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1333333333333333</v>
+        <v>0.8</v>
       </c>
       <c r="D20" t="n">
         <v>15</v>
@@ -991,14 +991,14 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>R_9emki3uWpm88jEt</t>
+          <t>R_9HiPuZ7ggaUWYXm</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>1.6</v>
+        <v>0.4</v>
       </c>
       <c r="D21" t="n">
         <v>15</v>
@@ -1018,14 +1018,14 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>R_9gLQpOlUhCZbZf0</t>
+          <t>R_4npneE7C0d2fzFf</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C22" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="D22" t="n">
         <v>15</v>
@@ -1045,14 +1045,14 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>R_91tsT1u49aBUhks</t>
+          <t>R_95Avzk7ufiikhMK</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D23" t="n">
         <v>15</v>
@@ -1072,14 +1072,14 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>R_9LAP8tEg6HUmoat</t>
+          <t>R_4QWwuNV77zEYamm</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>1.6</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D24" t="n">
         <v>15</v>
@@ -1099,14 +1099,14 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>R_4GCVAoEofofJmxX</t>
+          <t>R_4Nn2YPE5XSoLk77</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C25" t="n">
-        <v>0.7333333333333333</v>
+        <v>0.8</v>
       </c>
       <c r="D25" t="n">
         <v>15</v>
@@ -1126,14 +1126,14 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>R_4dtvPF6tKUsY2Dr</t>
+          <t>R_92mbrhLaUBLIZyA</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C26" t="n">
-        <v>0.8666666666666667</v>
+        <v>1.2</v>
       </c>
       <c r="D26" t="n">
         <v>15</v>
@@ -1153,14 +1153,14 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>R_9bTZgIxUTHOBB65</t>
+          <t>R_41tTqc4rClQAQ4c</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.6</v>
       </c>
       <c r="D27" t="n">
         <v>15</v>
@@ -1180,39 +1180,41 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>R_459tvSmsiMQmAJb</t>
+          <t>R_49TyR8AUyP9f0KR</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
-      </c>
-      <c r="C28" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E28" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
         <v>15</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>R_9GEAlR8ckucpR5i</t>
+          <t>R_99UYrIivDcdeF7r</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C29" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.8</v>
       </c>
       <c r="D29" t="n">
         <v>15</v>
@@ -1232,14 +1234,14 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>R_95AaIqXMdbZ4Fhr</t>
+          <t>R_9d0I0cLEUygFnzD</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>1.466666666666667</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="D30" t="n">
         <v>15</v>
@@ -1259,14 +1261,14 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>R_4lPSocYI5nk7Coh</t>
+          <t>R_47kRU4DvHWNnjGG</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C31" t="n">
-        <v>0.4666666666666667</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="D31" t="n">
         <v>15</v>
@@ -1286,39 +1288,41 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>R_4rHse7kHHEjzHly</t>
+          <t>R_9cj5AYT2isbQ025</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
-      </c>
-      <c r="C32" t="inlineStr"/>
+        <v>11</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.7333333333333333</v>
+      </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E32" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
         <v>15</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>R_4DYHJAe9FwcAbYM</t>
+          <t>R_96nUPcB7vcJX3jf</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C33" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.4</v>
       </c>
       <c r="D33" t="n">
         <v>15</v>
@@ -1338,14 +1342,14 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>R_4E1hPlVcrRYDEgI</t>
+          <t>R_4af1NjqrrNzcgut</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C34" t="n">
-        <v>0.8</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="D34" t="n">
         <v>15</v>
@@ -1365,14 +1369,14 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>R_9IrA4sK4uNKxOU1</t>
+          <t>R_9ctFQKbw2qIyZBw</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C35" t="n">
-        <v>0.7333333333333333</v>
+        <v>1.2</v>
       </c>
       <c r="D35" t="n">
         <v>15</v>
@@ -1392,39 +1396,41 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>R_4flYM0NAGQpPrrZ</t>
+          <t>R_4BsQya8zBjRULSx</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" t="inlineStr"/>
+        <v>6</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.4</v>
+      </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E36" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
         <v>15</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>R_9HiPuZ7ggaUWYXm</t>
+          <t>R_9UVGly5LAKAE4DH</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C37" t="n">
-        <v>0.4</v>
+        <v>1.133333333333333</v>
       </c>
       <c r="D37" t="n">
         <v>15</v>
@@ -1444,14 +1450,14 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>R_4npneE7C0d2fzFf</t>
+          <t>R_9hLtTGFf64ROzgA</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C38" t="n">
-        <v>0.2</v>
+        <v>1.2</v>
       </c>
       <c r="D38" t="n">
         <v>15</v>
@@ -1471,14 +1477,14 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>R_95Avzk7ufiikhMK</t>
+          <t>R_438xPgSQurWsGJ7</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C39" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6</v>
       </c>
       <c r="D39" t="n">
         <v>15</v>
@@ -1498,14 +1504,14 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>R_4QWwuNV77zEYamm</t>
+          <t>R_5EnHXfM9Ih1jcUw</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C40" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="D40" t="n">
         <v>15</v>
@@ -1525,14 +1531,14 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>R_4Nn2YPE5XSoLk77</t>
+          <t>R_4ooRca600URzSMF</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C41" t="n">
-        <v>0.8</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="D41" t="n">
         <v>15</v>
@@ -1552,14 +1558,14 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>R_92mbrhLaUBLIZyA</t>
+          <t>R_9z60gjDTdtBwz7i</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C42" t="n">
-        <v>1.2</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="D42" t="n">
         <v>15</v>
@@ -1579,14 +1585,14 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>R_4lCiksiXKcfJDNf</t>
+          <t>R_4z5hWHzjGPmlo3v</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C43" t="n">
-        <v>0.6</v>
+        <v>1.533333333333333</v>
       </c>
       <c r="D43" t="n">
         <v>15</v>
@@ -1606,14 +1612,14 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>R_41tTqc4rClQAQ4c</t>
+          <t>R_4R46XO9OwMarEXe</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C44" t="n">
-        <v>0.6</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="D44" t="n">
         <v>15</v>
@@ -1633,14 +1639,14 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>R_49TyR8AUyP9f0KR</t>
+          <t>R_4pyzOQaqk31zidB</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C45" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="D45" t="n">
         <v>15</v>
@@ -1660,14 +1666,14 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>R_99UYrIivDcdeF7r</t>
+          <t>R_9RXtm3TtL486t6z</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C46" t="n">
-        <v>0.8</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="D46" t="n">
         <v>15</v>
@@ -1679,241 +1685,6 @@
         <v>15</v>
       </c>
       <c r="G46" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>R_9d0I0cLEUygFnzD</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47" t="n">
-        <v>0.06666666666666667</v>
-      </c>
-      <c r="D47" t="n">
-        <v>15</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" t="n">
-        <v>15</v>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>R_425z6FKj0bv5S0N</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" t="n">
-        <v>15</v>
-      </c>
-      <c r="F48" t="n">
-        <v>15</v>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>R_9kBu3A4VzYEc7u4</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>0</v>
-      </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" t="n">
-        <v>15</v>
-      </c>
-      <c r="F49" t="n">
-        <v>15</v>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>R_47kRU4DvHWNnjGG</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>4</v>
-      </c>
-      <c r="C50" t="n">
-        <v>0.2666666666666667</v>
-      </c>
-      <c r="D50" t="n">
-        <v>15</v>
-      </c>
-      <c r="E50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" t="n">
-        <v>15</v>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>R_9cj5AYT2isbQ025</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>11</v>
-      </c>
-      <c r="C51" t="n">
-        <v>0.7333333333333333</v>
-      </c>
-      <c r="D51" t="n">
-        <v>15</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" t="n">
-        <v>15</v>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>R_4emUmach5eEaD7j</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>7</v>
-      </c>
-      <c r="C52" t="n">
-        <v>0.4666666666666667</v>
-      </c>
-      <c r="D52" t="n">
-        <v>15</v>
-      </c>
-      <c r="E52" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" t="n">
-        <v>15</v>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>R_4LTZEyvJAjeBq3o</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>0</v>
-      </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" t="n">
-        <v>15</v>
-      </c>
-      <c r="F53" t="n">
-        <v>15</v>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>R_9EoZrU2zlZGVxmh</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>0</v>
-      </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" t="n">
-        <v>15</v>
-      </c>
-      <c r="F54" t="n">
-        <v>15</v>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>R_9FLpP7aU380tJw8</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>12</v>
-      </c>
-      <c r="C55" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="D55" t="n">
-        <v>15</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" t="n">
-        <v>15</v>
-      </c>
-      <c r="G55" t="inlineStr">
         <is>
           <t>100.0%</t>
         </is>
@@ -1958,7 +1729,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>45</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1741,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>45</t>
         </is>
       </c>
     </row>
@@ -1982,7 +1753,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1998,7 +1769,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9.83</t>
+          <t>10.84</t>
         </is>
       </c>
     </row>
@@ -2010,7 +1781,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6.47</t>
+          <t>7.27</t>
         </is>
       </c>
     </row>
@@ -2022,7 +1793,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1.00</t>
         </is>
       </c>
     </row>
@@ -2062,7 +1833,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.66</t>
+          <t>0.72</t>
         </is>
       </c>
     </row>
@@ -2074,7 +1845,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.43</t>
+          <t>0.48</t>
         </is>
       </c>
     </row>
@@ -2086,7 +1857,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.07</t>
         </is>
       </c>
     </row>
@@ -2126,7 +1897,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>45</t>
         </is>
       </c>
     </row>
@@ -2153,7 +1924,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2201,14 +1972,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>R_42Ga7yjlA5oLJCd</t>
+          <t>R_4EEZWAH8SF10F8e</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5714285714285714</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="D2" t="n">
         <v>7</v>
@@ -2228,14 +1999,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>R_9j8Niq4DZA1y7Op</t>
+          <t>R_4AKE20ENCrCGxUl</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="D3" t="n">
         <v>7</v>
@@ -2255,14 +2026,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>R_92Xn58Elv9fCbLJ</t>
+          <t>R_9aZFWvCRMGokDwl</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>7</v>
@@ -2282,14 +2053,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>R_4pWgwYKsPFaTWcp</t>
+          <t>R_4eV7QBpawwD6eOr</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="D5" t="n">
         <v>7</v>
@@ -2309,14 +2080,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>R_4ELN7Q0714WIXDZ</t>
+          <t>R_91jRA37lX3YUEbP</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="D6" t="n">
         <v>7</v>
@@ -2336,14 +2107,14 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>R_9fPoQx2VAiJtvot</t>
+          <t>R_4PvVrWZ4ldg9ZuE</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1428571428571428</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
         <v>7</v>
@@ -2363,14 +2134,14 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>R_4EEZWAH8SF10F8e</t>
+          <t>R_9Y3cXt4ARx4xD6T</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>1.142857142857143</v>
+        <v>1.571428571428571</v>
       </c>
       <c r="D8" t="n">
         <v>7</v>
@@ -2390,14 +2161,14 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>R_4AKE20ENCrCGxUl</t>
+          <t>R_9N32winq5vbF1El</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7142857142857143</v>
+        <v>1.571428571428571</v>
       </c>
       <c r="D9" t="n">
         <v>7</v>
@@ -2417,14 +2188,14 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>R_9aZFWvCRMGokDwl</t>
+          <t>R_9uYGNjx9yWaODxD</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
         <v>7</v>
@@ -2444,14 +2215,14 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>R_4eV7QBpawwD6eOr</t>
+          <t>R_9OPvlHXlbPmz754</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="D11" t="n">
         <v>7</v>
@@ -2471,14 +2242,14 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>R_91jRA37lX3YUEbP</t>
+          <t>R_9x36NNwdNT2QnEB</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2857142857142857</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
         <v>7</v>
@@ -2498,14 +2269,14 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>R_4PvVrWZ4ldg9ZuE</t>
+          <t>R_4DfI1n39Bzpi2xH</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="D13" t="n">
         <v>7</v>
@@ -2525,14 +2296,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>R_9Y3cXt4ARx4xD6T</t>
+          <t>R_9emki3uWpm88jEt</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C14" t="n">
-        <v>1.571428571428571</v>
+        <v>2.571428571428572</v>
       </c>
       <c r="D14" t="n">
         <v>7</v>
@@ -2552,14 +2323,14 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>R_9N32winq5vbF1El</t>
+          <t>R_91tsT1u49aBUhks</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C15" t="n">
-        <v>1.571428571428571</v>
+        <v>2.142857142857143</v>
       </c>
       <c r="D15" t="n">
         <v>7</v>
@@ -2579,14 +2350,14 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>R_9uYGNjx9yWaODxD</t>
+          <t>R_9LAP8tEg6HUmoat</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="D16" t="n">
         <v>7</v>
@@ -2606,14 +2377,14 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>R_9OPvlHXlbPmz754</t>
+          <t>R_4GCVAoEofofJmxX</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1428571428571428</v>
+        <v>1.714285714285714</v>
       </c>
       <c r="D17" t="n">
         <v>7</v>
@@ -2633,14 +2404,14 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>R_4rHDTNQ0TLPg3iz</t>
+          <t>R_4dtvPF6tKUsY2Dr</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="D18" t="n">
         <v>7</v>
@@ -2660,14 +2431,14 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>R_9x36NNwdNT2QnEB</t>
+          <t>R_9bTZgIxUTHOBB65</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="D19" t="n">
         <v>7</v>
@@ -2687,14 +2458,14 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>R_4DfI1n39Bzpi2xH</t>
+          <t>R_4E1hPlVcrRYDEgI</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1428571428571428</v>
+        <v>2</v>
       </c>
       <c r="D20" t="n">
         <v>7</v>
@@ -2714,14 +2485,14 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>R_9emki3uWpm88jEt</t>
+          <t>R_9HiPuZ7ggaUWYXm</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C21" t="n">
-        <v>2.571428571428572</v>
+        <v>1.428571428571429</v>
       </c>
       <c r="D21" t="n">
         <v>7</v>
@@ -2741,14 +2512,14 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>R_9gLQpOlUhCZbZf0</t>
+          <t>R_4npneE7C0d2fzFf</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>7</v>
@@ -2768,14 +2539,14 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>R_91tsT1u49aBUhks</t>
+          <t>R_95Avzk7ufiikhMK</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>2.142857142857143</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="D23" t="n">
         <v>7</v>
@@ -2795,14 +2566,14 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>R_9LAP8tEg6HUmoat</t>
+          <t>R_4QWwuNV77zEYamm</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8571428571428571</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
         <v>7</v>
@@ -2822,14 +2593,14 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>R_4GCVAoEofofJmxX</t>
+          <t>R_4Nn2YPE5XSoLk77</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C25" t="n">
-        <v>1.714285714285714</v>
+        <v>1.857142857142857</v>
       </c>
       <c r="D25" t="n">
         <v>7</v>
@@ -2849,14 +2620,14 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>R_4dtvPF6tKUsY2Dr</t>
+          <t>R_92mbrhLaUBLIZyA</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C26" t="n">
-        <v>0.7142857142857143</v>
+        <v>1.428571428571429</v>
       </c>
       <c r="D26" t="n">
         <v>7</v>
@@ -2876,14 +2647,14 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>R_9bTZgIxUTHOBB65</t>
+          <t>R_41tTqc4rClQAQ4c</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C27" t="n">
-        <v>1.142857142857143</v>
+        <v>1.714285714285714</v>
       </c>
       <c r="D27" t="n">
         <v>7</v>
@@ -2903,32 +2674,34 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>R_459tvSmsiMQmAJb</t>
+          <t>R_49TyR8AUyP9f0KR</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
-      </c>
-      <c r="C28" t="inlineStr"/>
+        <v>11</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1.571428571428571</v>
+      </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
         <v>7</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>R_9GEAlR8ckucpR5i</t>
+          <t>R_99UYrIivDcdeF7r</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -2955,14 +2728,14 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>R_95AaIqXMdbZ4Fhr</t>
+          <t>R_9d0I0cLEUygFnzD</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>2.571428571428572</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
         <v>7</v>
@@ -2982,14 +2755,14 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>R_4lPSocYI5nk7Coh</t>
+          <t>R_47kRU4DvHWNnjGG</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C31" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="D31" t="n">
         <v>7</v>
@@ -3009,39 +2782,41 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>R_4rHse7kHHEjzHly</t>
+          <t>R_9cj5AYT2isbQ025</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
-      </c>
-      <c r="C32" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E32" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
         <v>7</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>R_4DYHJAe9FwcAbYM</t>
+          <t>R_96nUPcB7vcJX3jf</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C33" t="n">
-        <v>1.285714285714286</v>
+        <v>1.571428571428571</v>
       </c>
       <c r="D33" t="n">
         <v>7</v>
@@ -3061,14 +2836,14 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>R_4E1hPlVcrRYDEgI</t>
+          <t>R_4af1NjqrrNzcgut</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C34" t="n">
-        <v>2</v>
+        <v>2.571428571428572</v>
       </c>
       <c r="D34" t="n">
         <v>7</v>
@@ -3088,14 +2863,14 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>R_9IrA4sK4uNKxOU1</t>
+          <t>R_9ctFQKbw2qIyZBw</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C35" t="n">
-        <v>1.428571428571429</v>
+        <v>1.714285714285714</v>
       </c>
       <c r="D35" t="n">
         <v>7</v>
@@ -3115,39 +2890,41 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>R_4flYM0NAGQpPrrZ</t>
+          <t>R_4BsQya8zBjRULSx</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.5714285714285714</v>
+      </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E36" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
         <v>7</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>R_9HiPuZ7ggaUWYXm</t>
+          <t>R_9UVGly5LAKAE4DH</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C37" t="n">
-        <v>1.428571428571429</v>
+        <v>1.714285714285714</v>
       </c>
       <c r="D37" t="n">
         <v>7</v>
@@ -3167,14 +2944,14 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>R_4npneE7C0d2fzFf</t>
+          <t>R_9hLtTGFf64ROzgA</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1.714285714285714</v>
       </c>
       <c r="D38" t="n">
         <v>7</v>
@@ -3194,14 +2971,14 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>R_95Avzk7ufiikhMK</t>
+          <t>R_438xPgSQurWsGJ7</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C39" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="D39" t="n">
         <v>7</v>
@@ -3221,14 +2998,14 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>R_4QWwuNV77zEYamm</t>
+          <t>R_5EnHXfM9Ih1jcUw</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="D40" t="n">
         <v>7</v>
@@ -3248,14 +3025,14 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>R_4Nn2YPE5XSoLk77</t>
+          <t>R_4ooRca600URzSMF</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C41" t="n">
-        <v>1.857142857142857</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
         <v>7</v>
@@ -3275,14 +3052,14 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>R_92mbrhLaUBLIZyA</t>
+          <t>R_9z60gjDTdtBwz7i</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C42" t="n">
-        <v>1.428571428571429</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="D42" t="n">
         <v>7</v>
@@ -3302,14 +3079,14 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>R_4lCiksiXKcfJDNf</t>
+          <t>R_4z5hWHzjGPmlo3v</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>0.8571428571428571</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
         <v>7</v>
@@ -3329,14 +3106,14 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>R_41tTqc4rClQAQ4c</t>
+          <t>R_4R46XO9OwMarEXe</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>1.714285714285714</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
         <v>7</v>
@@ -3356,14 +3133,14 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>R_49TyR8AUyP9f0KR</t>
+          <t>R_4pyzOQaqk31zidB</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>1.571428571428571</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
         <v>7</v>
@@ -3383,14 +3160,14 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>R_99UYrIivDcdeF7r</t>
+          <t>R_9RXtm3TtL486t6z</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C46" t="n">
-        <v>1.142857142857143</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="D46" t="n">
         <v>7</v>
@@ -3402,241 +3179,6 @@
         <v>7</v>
       </c>
       <c r="G46" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>R_9d0I0cLEUygFnzD</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>0</v>
-      </c>
-      <c r="C47" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" t="n">
-        <v>7</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" t="n">
-        <v>7</v>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>R_425z6FKj0bv5S0N</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" t="n">
-        <v>7</v>
-      </c>
-      <c r="F48" t="n">
-        <v>7</v>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>R_9kBu3A4VzYEc7u4</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>0</v>
-      </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" t="n">
-        <v>7</v>
-      </c>
-      <c r="F49" t="n">
-        <v>7</v>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>R_47kRU4DvHWNnjGG</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>2</v>
-      </c>
-      <c r="C50" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="D50" t="n">
-        <v>7</v>
-      </c>
-      <c r="E50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" t="n">
-        <v>7</v>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>R_9cj5AYT2isbQ025</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>7</v>
-      </c>
-      <c r="C51" t="n">
-        <v>1</v>
-      </c>
-      <c r="D51" t="n">
-        <v>7</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" t="n">
-        <v>7</v>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>R_4emUmach5eEaD7j</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>3</v>
-      </c>
-      <c r="C52" t="n">
-        <v>0.4285714285714285</v>
-      </c>
-      <c r="D52" t="n">
-        <v>7</v>
-      </c>
-      <c r="E52" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" t="n">
-        <v>7</v>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>R_4LTZEyvJAjeBq3o</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>0</v>
-      </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" t="n">
-        <v>7</v>
-      </c>
-      <c r="F53" t="n">
-        <v>7</v>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>R_9EoZrU2zlZGVxmh</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>0</v>
-      </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" t="n">
-        <v>7</v>
-      </c>
-      <c r="F54" t="n">
-        <v>7</v>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>R_9FLpP7aU380tJw8</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>6</v>
-      </c>
-      <c r="C55" t="n">
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="D55" t="n">
-        <v>7</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" t="n">
-        <v>7</v>
-      </c>
-      <c r="G55" t="inlineStr">
         <is>
           <t>100.0%</t>
         </is>
@@ -3681,7 +3223,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>45</t>
         </is>
       </c>
     </row>
@@ -3693,7 +3235,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>45</t>
         </is>
       </c>
     </row>
@@ -3705,7 +3247,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3721,7 +3263,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>7.55</t>
+          <t>7.49</t>
         </is>
       </c>
     </row>
@@ -3733,7 +3275,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5.01</t>
+          <t>5.34</t>
         </is>
       </c>
     </row>
@@ -3785,7 +3327,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1.08</t>
+          <t>1.07</t>
         </is>
       </c>
     </row>
@@ -3797,7 +3339,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.72</t>
+          <t>0.76</t>
         </is>
       </c>
     </row>
@@ -3849,7 +3391,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>45</t>
         </is>
       </c>
     </row>
@@ -3876,7 +3418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3944,23 +3486,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>R_42Ga7yjlA5oLJCd</t>
+          <t>R_4EEZWAH8SF10F8e</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="n">
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G2" t="n">
         <v>8</v>
@@ -3983,23 +3525,23 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>R_9j8Niq4DZA1y7Op</t>
+          <t>R_4AKE20ENCrCGxUl</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C3" t="n">
         <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E3" t="n">
         <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G3" t="n">
         <v>8</v>
@@ -4022,23 +3564,23 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>R_92Xn58Elv9fCbLJ</t>
+          <t>R_9aZFWvCRMGokDwl</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
         <v>8</v>
       </c>
       <c r="D4" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E4" t="n">
         <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4" t="n">
         <v>8</v>
@@ -4061,62 +3603,62 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>R_4pWgwYKsPFaTWcp</t>
+          <t>R_4eV7QBpawwD6eOr</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E5" t="n">
         <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G5" t="n">
         <v>8</v>
       </c>
       <c r="H5" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
         <v>26</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>96.2%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>R_4ELN7Q0714WIXDZ</t>
+          <t>R_91jRA37lX3YUEbP</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" t="n">
         <v>8</v>
       </c>
       <c r="D6" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
         <v>10</v>
       </c>
       <c r="F6" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G6" t="n">
         <v>8</v>
@@ -4139,62 +3681,62 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>R_9fPoQx2VAiJtvot</t>
+          <t>R_4PvVrWZ4ldg9ZuE</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C7" t="n">
         <v>8</v>
       </c>
       <c r="D7" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E7" t="n">
         <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
         <v>26</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>96.2%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>R_4EEZWAH8SF10F8e</t>
+          <t>R_9Y3cXt4ARx4xD6T</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="n">
         <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E8" t="n">
         <v>10</v>
       </c>
       <c r="F8" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G8" t="n">
         <v>8</v>
@@ -4217,23 +3759,23 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>R_4AKE20ENCrCGxUl</t>
+          <t>R_9N32winq5vbF1El</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E9" t="n">
         <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G9" t="n">
         <v>8</v>
@@ -4256,23 +3798,23 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>R_9aZFWvCRMGokDwl</t>
+          <t>R_9uYGNjx9yWaODxD</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C10" t="n">
         <v>8</v>
       </c>
       <c r="D10" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E10" t="n">
         <v>10</v>
       </c>
       <c r="F10" t="n">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="G10" t="n">
         <v>8</v>
@@ -4295,62 +3837,62 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>R_4eV7QBpawwD6eOr</t>
+          <t>R_9OPvlHXlbPmz754</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E11" t="n">
         <v>10</v>
       </c>
       <c r="F11" t="n">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="G11" t="n">
         <v>8</v>
       </c>
       <c r="H11" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
         <v>26</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>96.2%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>R_91jRA37lX3YUEbP</t>
+          <t>R_9x36NNwdNT2QnEB</t>
         </is>
       </c>
       <c r="B12" t="n">
+        <v>17</v>
+      </c>
+      <c r="C12" t="n">
+        <v>8</v>
+      </c>
+      <c r="D12" t="n">
         <v>12</v>
       </c>
-      <c r="C12" t="n">
-        <v>8</v>
-      </c>
-      <c r="D12" t="n">
-        <v>10</v>
-      </c>
       <c r="E12" t="n">
         <v>10</v>
       </c>
       <c r="F12" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G12" t="n">
         <v>8</v>
@@ -4373,62 +3915,62 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>R_4PvVrWZ4ldg9ZuE</t>
+          <t>R_4DfI1n39Bzpi2xH</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C13" t="n">
         <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="E13" t="n">
         <v>10</v>
       </c>
       <c r="F13" t="n">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G13" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H13" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
         <v>26</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>96.2%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>R_9Y3cXt4ARx4xD6T</t>
+          <t>R_9emki3uWpm88jEt</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C14" t="n">
         <v>8</v>
       </c>
       <c r="D14" t="n">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="E14" t="n">
         <v>10</v>
       </c>
       <c r="F14" t="n">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="G14" t="n">
         <v>8</v>
@@ -4451,23 +3993,23 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>R_9N32winq5vbF1El</t>
+          <t>R_91tsT1u49aBUhks</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C15" t="n">
         <v>8</v>
       </c>
       <c r="D15" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E15" t="n">
         <v>10</v>
       </c>
       <c r="F15" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G15" t="n">
         <v>8</v>
@@ -4490,23 +4032,23 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>R_9uYGNjx9yWaODxD</t>
+          <t>R_9LAP8tEg6HUmoat</t>
         </is>
       </c>
       <c r="B16" t="n">
+        <v>19</v>
+      </c>
+      <c r="C16" t="n">
+        <v>8</v>
+      </c>
+      <c r="D16" t="n">
+        <v>17</v>
+      </c>
+      <c r="E16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" t="n">
         <v>34</v>
-      </c>
-      <c r="C16" t="n">
-        <v>8</v>
-      </c>
-      <c r="D16" t="n">
-        <v>16</v>
-      </c>
-      <c r="E16" t="n">
-        <v>10</v>
-      </c>
-      <c r="F16" t="n">
-        <v>39</v>
       </c>
       <c r="G16" t="n">
         <v>8</v>
@@ -4529,23 +4071,23 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>R_9OPvlHXlbPmz754</t>
+          <t>R_4GCVAoEofofJmxX</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C17" t="n">
         <v>8</v>
       </c>
       <c r="D17" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E17" t="n">
         <v>10</v>
       </c>
       <c r="F17" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G17" t="n">
         <v>8</v>
@@ -4568,11 +4110,11 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>R_4rHDTNQ0TLPg3iz</t>
+          <t>R_4dtvPF6tKUsY2Dr</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C18" t="n">
         <v>8</v>
@@ -4584,7 +4126,7 @@
         <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G18" t="n">
         <v>8</v>
@@ -4607,23 +4149,23 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>R_9x36NNwdNT2QnEB</t>
+          <t>R_9bTZgIxUTHOBB65</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C19" t="n">
         <v>8</v>
       </c>
       <c r="D19" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E19" t="n">
         <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G19" t="n">
         <v>8</v>
@@ -4646,23 +4188,23 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>R_4DfI1n39Bzpi2xH</t>
+          <t>R_4E1hPlVcrRYDEgI</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C20" t="n">
         <v>8</v>
       </c>
       <c r="D20" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E20" t="n">
         <v>10</v>
       </c>
       <c r="F20" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G20" t="n">
         <v>8</v>
@@ -4685,23 +4227,23 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>R_9emki3uWpm88jEt</t>
+          <t>R_9HiPuZ7ggaUWYXm</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C21" t="n">
         <v>8</v>
       </c>
       <c r="D21" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E21" t="n">
         <v>10</v>
       </c>
       <c r="F21" t="n">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="G21" t="n">
         <v>8</v>
@@ -4724,23 +4266,23 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>R_9gLQpOlUhCZbZf0</t>
+          <t>R_4npneE7C0d2fzFf</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C22" t="n">
         <v>8</v>
       </c>
       <c r="D22" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E22" t="n">
         <v>10</v>
       </c>
       <c r="F22" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G22" t="n">
         <v>8</v>
@@ -4763,23 +4305,23 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>R_91tsT1u49aBUhks</t>
+          <t>R_95Avzk7ufiikhMK</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C23" t="n">
         <v>8</v>
       </c>
       <c r="D23" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E23" t="n">
         <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G23" t="n">
         <v>8</v>
@@ -4802,23 +4344,23 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>R_9LAP8tEg6HUmoat</t>
+          <t>R_4QWwuNV77zEYamm</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C24" t="n">
         <v>8</v>
       </c>
       <c r="D24" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E24" t="n">
         <v>10</v>
       </c>
       <c r="F24" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G24" t="n">
         <v>8</v>
@@ -4841,23 +4383,23 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>R_4GCVAoEofofJmxX</t>
+          <t>R_4Nn2YPE5XSoLk77</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C25" t="n">
         <v>8</v>
       </c>
       <c r="D25" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E25" t="n">
         <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G25" t="n">
         <v>8</v>
@@ -4880,23 +4422,23 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>R_4dtvPF6tKUsY2Dr</t>
+          <t>R_92mbrhLaUBLIZyA</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C26" t="n">
         <v>8</v>
       </c>
       <c r="D26" t="n">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E26" t="n">
         <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G26" t="n">
         <v>8</v>
@@ -4919,23 +4461,23 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>R_9bTZgIxUTHOBB65</t>
+          <t>R_41tTqc4rClQAQ4c</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" t="n">
         <v>8</v>
       </c>
       <c r="D27" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E27" t="n">
         <v>10</v>
       </c>
       <c r="F27" t="n">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G27" t="n">
         <v>8</v>
@@ -4958,62 +4500,62 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>R_459tvSmsiMQmAJb</t>
+          <t>R_49TyR8AUyP9f0KR</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="I28" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="J28" t="n">
         <v>26</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>R_9GEAlR8ckucpR5i</t>
+          <t>R_99UYrIivDcdeF7r</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C29" t="n">
         <v>8</v>
       </c>
       <c r="D29" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E29" t="n">
         <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G29" t="n">
         <v>8</v>
@@ -5036,23 +4578,23 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>R_95AaIqXMdbZ4Fhr</t>
+          <t>R_9d0I0cLEUygFnzD</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="C30" t="n">
         <v>8</v>
       </c>
       <c r="D30" t="n">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E30" t="n">
         <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G30" t="n">
         <v>8</v>
@@ -5075,23 +4617,23 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>R_4lPSocYI5nk7Coh</t>
+          <t>R_47kRU4DvHWNnjGG</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C31" t="n">
         <v>8</v>
       </c>
       <c r="D31" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E31" t="n">
         <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G31" t="n">
         <v>8</v>
@@ -5114,62 +4656,62 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>R_4rHse7kHHEjzHly</t>
+          <t>R_9cj5AYT2isbQ025</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="I32" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="J32" t="n">
         <v>26</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>R_4DYHJAe9FwcAbYM</t>
+          <t>R_96nUPcB7vcJX3jf</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33" t="n">
         <v>8</v>
       </c>
       <c r="D33" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E33" t="n">
         <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G33" t="n">
         <v>8</v>
@@ -5192,23 +4734,23 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>R_4E1hPlVcrRYDEgI</t>
+          <t>R_4af1NjqrrNzcgut</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C34" t="n">
         <v>8</v>
       </c>
       <c r="D34" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E34" t="n">
         <v>10</v>
       </c>
       <c r="F34" t="n">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="G34" t="n">
         <v>8</v>
@@ -5231,23 +4773,23 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>R_9IrA4sK4uNKxOU1</t>
+          <t>R_9ctFQKbw2qIyZBw</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C35" t="n">
         <v>8</v>
       </c>
       <c r="D35" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E35" t="n">
         <v>10</v>
       </c>
       <c r="F35" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G35" t="n">
         <v>8</v>
@@ -5270,62 +4812,62 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>R_4flYM0NAGQpPrrZ</t>
+          <t>R_4BsQya8zBjRULSx</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="I36" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="J36" t="n">
         <v>26</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>R_9HiPuZ7ggaUWYXm</t>
+          <t>R_9UVGly5LAKAE4DH</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C37" t="n">
         <v>8</v>
       </c>
       <c r="D37" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E37" t="n">
         <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G37" t="n">
         <v>8</v>
@@ -5348,50 +4890,50 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>R_4npneE7C0d2fzFf</t>
+          <t>R_9hLtTGFf64ROzgA</t>
         </is>
       </c>
       <c r="B38" t="n">
+        <v>26</v>
+      </c>
+      <c r="C38" t="n">
+        <v>8</v>
+      </c>
+      <c r="D38" t="n">
         <v>11</v>
       </c>
-      <c r="C38" t="n">
-        <v>8</v>
-      </c>
-      <c r="D38" t="n">
-        <v>10</v>
-      </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G38" t="n">
         <v>8</v>
       </c>
       <c r="H38" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="n">
         <v>26</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>96.2%</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>R_95Avzk7ufiikhMK</t>
+          <t>R_438xPgSQurWsGJ7</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C39" t="n">
         <v>8</v>
@@ -5403,7 +4945,7 @@
         <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G39" t="n">
         <v>8</v>
@@ -5426,23 +4968,23 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>R_4QWwuNV77zEYamm</t>
+          <t>R_5EnHXfM9Ih1jcUw</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40" t="n">
         <v>8</v>
       </c>
       <c r="D40" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E40" t="n">
         <v>10</v>
       </c>
       <c r="F40" t="n">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="G40" t="n">
         <v>8</v>
@@ -5465,23 +5007,23 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>R_4Nn2YPE5XSoLk77</t>
+          <t>R_4ooRca600URzSMF</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C41" t="n">
         <v>8</v>
       </c>
       <c r="D41" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E41" t="n">
         <v>10</v>
       </c>
       <c r="F41" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G41" t="n">
         <v>8</v>
@@ -5504,17 +5046,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>R_92mbrhLaUBLIZyA</t>
+          <t>R_9z60gjDTdtBwz7i</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C42" t="n">
         <v>8</v>
       </c>
       <c r="D42" t="n">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E42" t="n">
         <v>10</v>
@@ -5543,14 +5085,14 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>R_4lCiksiXKcfJDNf</t>
+          <t>R_4z5hWHzjGPmlo3v</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D43" t="n">
         <v>17</v>
@@ -5559,46 +5101,46 @@
         <v>10</v>
       </c>
       <c r="F43" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G43" t="n">
         <v>8</v>
       </c>
       <c r="H43" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="n">
         <v>26</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>96.2%</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>R_41tTqc4rClQAQ4c</t>
+          <t>R_4R46XO9OwMarEXe</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C44" t="n">
         <v>8</v>
       </c>
       <c r="D44" t="n">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="E44" t="n">
         <v>10</v>
       </c>
       <c r="F44" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G44" t="n">
         <v>8</v>
@@ -5621,23 +5163,23 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>R_49TyR8AUyP9f0KR</t>
+          <t>R_4pyzOQaqk31zidB</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C45" t="n">
         <v>8</v>
       </c>
       <c r="D45" t="n">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E45" t="n">
         <v>10</v>
       </c>
       <c r="F45" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G45" t="n">
         <v>8</v>
@@ -5660,23 +5202,23 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>R_99UYrIivDcdeF7r</t>
+          <t>R_9RXtm3TtL486t6z</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C46" t="n">
         <v>8</v>
       </c>
       <c r="D46" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E46" t="n">
         <v>10</v>
       </c>
       <c r="F46" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G46" t="n">
         <v>8</v>
@@ -5691,357 +5233,6 @@
         <v>26</v>
       </c>
       <c r="K46" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>R_9d0I0cLEUygFnzD</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>9</v>
-      </c>
-      <c r="C47" t="n">
-        <v>8</v>
-      </c>
-      <c r="D47" t="n">
-        <v>10</v>
-      </c>
-      <c r="E47" t="n">
-        <v>10</v>
-      </c>
-      <c r="F47" t="n">
-        <v>23</v>
-      </c>
-      <c r="G47" t="n">
-        <v>8</v>
-      </c>
-      <c r="H47" t="n">
-        <v>26</v>
-      </c>
-      <c r="I47" t="n">
-        <v>0</v>
-      </c>
-      <c r="J47" t="n">
-        <v>26</v>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>R_425z6FKj0bv5S0N</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C48" t="n">
-        <v>0</v>
-      </c>
-      <c r="D48" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0</v>
-      </c>
-      <c r="H48" t="n">
-        <v>0</v>
-      </c>
-      <c r="I48" t="n">
-        <v>26</v>
-      </c>
-      <c r="J48" t="n">
-        <v>26</v>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>R_9kBu3A4VzYEc7u4</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>0</v>
-      </c>
-      <c r="C49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" t="n">
-        <v>0</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0</v>
-      </c>
-      <c r="I49" t="n">
-        <v>26</v>
-      </c>
-      <c r="J49" t="n">
-        <v>26</v>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>R_47kRU4DvHWNnjGG</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>12</v>
-      </c>
-      <c r="C50" t="n">
-        <v>8</v>
-      </c>
-      <c r="D50" t="n">
-        <v>14</v>
-      </c>
-      <c r="E50" t="n">
-        <v>10</v>
-      </c>
-      <c r="F50" t="n">
-        <v>17</v>
-      </c>
-      <c r="G50" t="n">
-        <v>8</v>
-      </c>
-      <c r="H50" t="n">
-        <v>26</v>
-      </c>
-      <c r="I50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J50" t="n">
-        <v>26</v>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>R_9cj5AYT2isbQ025</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>18</v>
-      </c>
-      <c r="C51" t="n">
-        <v>8</v>
-      </c>
-      <c r="D51" t="n">
-        <v>13</v>
-      </c>
-      <c r="E51" t="n">
-        <v>10</v>
-      </c>
-      <c r="F51" t="n">
-        <v>27</v>
-      </c>
-      <c r="G51" t="n">
-        <v>8</v>
-      </c>
-      <c r="H51" t="n">
-        <v>26</v>
-      </c>
-      <c r="I51" t="n">
-        <v>0</v>
-      </c>
-      <c r="J51" t="n">
-        <v>26</v>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>R_4emUmach5eEaD7j</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>26</v>
-      </c>
-      <c r="C52" t="n">
-        <v>8</v>
-      </c>
-      <c r="D52" t="n">
-        <v>21</v>
-      </c>
-      <c r="E52" t="n">
-        <v>10</v>
-      </c>
-      <c r="F52" t="n">
-        <v>30</v>
-      </c>
-      <c r="G52" t="n">
-        <v>8</v>
-      </c>
-      <c r="H52" t="n">
-        <v>26</v>
-      </c>
-      <c r="I52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J52" t="n">
-        <v>26</v>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>R_4LTZEyvJAjeBq3o</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>0</v>
-      </c>
-      <c r="C53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" t="n">
-        <v>0</v>
-      </c>
-      <c r="G53" t="n">
-        <v>0</v>
-      </c>
-      <c r="H53" t="n">
-        <v>0</v>
-      </c>
-      <c r="I53" t="n">
-        <v>26</v>
-      </c>
-      <c r="J53" t="n">
-        <v>26</v>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>R_9EoZrU2zlZGVxmh</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>0</v>
-      </c>
-      <c r="C54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0</v>
-      </c>
-      <c r="H54" t="n">
-        <v>0</v>
-      </c>
-      <c r="I54" t="n">
-        <v>26</v>
-      </c>
-      <c r="J54" t="n">
-        <v>26</v>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>R_9FLpP7aU380tJw8</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>22</v>
-      </c>
-      <c r="C55" t="n">
-        <v>8</v>
-      </c>
-      <c r="D55" t="n">
-        <v>16</v>
-      </c>
-      <c r="E55" t="n">
-        <v>10</v>
-      </c>
-      <c r="F55" t="n">
-        <v>24</v>
-      </c>
-      <c r="G55" t="n">
-        <v>8</v>
-      </c>
-      <c r="H55" t="n">
-        <v>26</v>
-      </c>
-      <c r="I55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J55" t="n">
-        <v>26</v>
-      </c>
-      <c r="K55" t="inlineStr">
         <is>
           <t>100.0%</t>
         </is>
@@ -6086,7 +5277,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>45</t>
         </is>
       </c>
     </row>
@@ -6098,7 +5289,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>45</t>
         </is>
       </c>
     </row>
@@ -6110,7 +5301,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -6122,7 +5313,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>99.8%</t>
+          <t>99.7%</t>
         </is>
       </c>
     </row>
@@ -6138,7 +5329,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>18.83</t>
+          <t>18.16</t>
         </is>
       </c>
     </row>
@@ -6150,7 +5341,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7.68</t>
+          <t>7.98</t>
         </is>
       </c>
     </row>
@@ -6174,7 +5365,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>39.00</t>
+          <t>38.00</t>
         </is>
       </c>
     </row>
@@ -6186,7 +5377,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>18.00</t>
+          <t>16.00</t>
         </is>
       </c>
     </row>
@@ -6202,7 +5393,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>19.00</t>
+          <t>16.91</t>
         </is>
       </c>
     </row>
@@ -6214,7 +5405,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>8.21</t>
+          <t>7.78</t>
         </is>
       </c>
     </row>
@@ -6250,7 +5441,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>17.00</t>
+          <t>15.00</t>
         </is>
       </c>
     </row>
@@ -6266,7 +5457,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>26.21</t>
+          <t>26.49</t>
         </is>
       </c>
     </row>
@@ -6278,7 +5469,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5.32</t>
+          <t>6.23</t>
         </is>
       </c>
     </row>
@@ -6290,7 +5481,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>15.00</t>
+          <t>12.00</t>
         </is>
       </c>
     </row>
@@ -6314,7 +5505,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>26.00</t>
+          <t>27.00</t>
         </is>
       </c>
     </row>

</xml_diff>